<commit_message>
Modified generateAgesAtDeath function to allow for an adjustment in years (the adjustment is added to the result).   This required adding such an input to each person.  Also, there's an option to randomize the order of the output.
Cash flows can now use a defaultInflation rate for the the simulation or a rate specific to the cash flow.
</commit_message>
<xml_diff>
--- a/inst/extdata/siminput.xlsx
+++ b/inst/extdata/siminput.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rex\Documents\AA\aasim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b1bc217bf759e6b/aasim/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_86886DA4862F4F2112852ABA20DD14779D22FE25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C80C0A-C101-4869-AFB7-154D41786B18}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="57480" yWindow="6405" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="cashflows" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>nTrials</t>
   </si>
@@ -42,9 +43,6 @@
     <t>seed</t>
   </si>
   <si>
-    <t>inflation</t>
-  </si>
-  <si>
     <t>ror</t>
   </si>
   <si>
@@ -138,9 +136,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>inflationadj</t>
-  </si>
-  <si>
     <t>yr</t>
   </si>
   <si>
@@ -181,12 +176,27 @@
   </si>
   <si>
     <t>simulation</t>
+  </si>
+  <si>
+    <t>defaultInflation</t>
+  </si>
+  <si>
+    <t>p1mortadjyears</t>
+  </si>
+  <si>
+    <t>p2mortadjyears</t>
+  </si>
+  <si>
+    <t>defaultInflationadj</t>
+  </si>
+  <si>
+    <t>Inflation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -497,22 +507,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -529,60 +539,66 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -591,7 +607,7 @@
         <v>1000000</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>101</v>
@@ -612,16 +628,16 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
       </c>
       <c r="M2">
         <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2">
         <v>65</v>
@@ -629,10 +645,16 @@
       <c r="P2">
         <v>1</v>
       </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -641,7 +663,7 @@
         <v>1000000</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>101</v>
@@ -662,16 +684,16 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
       </c>
       <c r="M3">
         <v>56</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <v>65</v>
@@ -679,23 +701,29 @@
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" t="s">
         <v>28</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3">
+        <v>53</v>
+      </c>
+      <c r="U3" t="s">
         <v>29</v>
       </c>
-      <c r="S3">
-        <v>53</v>
-      </c>
-      <c r="T3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3">
+      <c r="V3">
         <v>65</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -704,66 +732,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
       <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
       </c>
       <c r="H2">
         <v>20000</v>
@@ -771,28 +802,31 @@
       <c r="I2" t="b">
         <v>0</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>5000</v>
@@ -800,28 +834,31 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4">
         <v>500</v>
@@ -829,28 +866,31 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5">
         <v>50</v>
@@ -858,28 +898,31 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>10000</v>
@@ -887,33 +930,39 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
       </c>
       <c r="H7">
         <v>20000</v>
       </c>
       <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>0</v>
       </c>
     </row>

</xml_diff>